<commit_message>
updates made to GUI and normalized scores for easy reading
</commit_message>
<xml_diff>
--- a/who_test_controls.xlsx
+++ b/who_test_controls.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee8d3d5c28cf10e6/Desktop/final_consolidated_analyzer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_F30EBDCA97D9AECF8A160B23FB64D1F260120287" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA15859-C852-49C8-9C1C-32B2A32BB4D9}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Control_ID</t>
   </si>
@@ -65,13 +71,31 @@
   </si>
   <si>
     <t>Preventive</t>
+  </si>
+  <si>
+    <t>Audit Leader</t>
+  </si>
+  <si>
+    <t>Triple H</t>
+  </si>
+  <si>
+    <t>TripleH</t>
+  </si>
+  <si>
+    <t>The Rock</t>
+  </si>
+  <si>
+    <t>Undertaker</t>
+  </si>
+  <si>
+    <t>Mankind</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,13 +158,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +210,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -212,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -246,9 +279,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,136 +455,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
         <v>12651</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
         <v>11102</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
         <v>6463</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
         <v>7140</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
         <v>10575</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
         <v>4645</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
         <v>4310</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
         <v>3867</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed files to reference column mapping appropriately.
</commit_message>
<xml_diff>
--- a/who_test_controls.xlsx
+++ b/who_test_controls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee8d3d5c28cf10e6/Desktop/final_consolidated_analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F30EBDCA97D9AECF8A160B23FB64D1F260120287" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA15859-C852-49C8-9C1C-32B2A32BB4D9}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_F30EBDCA97D9AECF8A160B23FB64D1F260120287" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF279D33-FB0A-4962-B33E-FB50BE1F5361}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,18 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
-    <t>Control_ID</t>
-  </si>
-  <si>
-    <t>Control_Description</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Control_Type</t>
-  </si>
-  <si>
     <t>On a monthly basis, the Global Card Issuance (GCI) team monitors the production queue to ensure all customer cards are issued within SLA timelines.</t>
   </si>
   <si>
@@ -73,9 +61,6 @@
     <t>Preventive</t>
   </si>
   <si>
-    <t>Audit Leader</t>
-  </si>
-  <si>
     <t>Triple H</t>
   </si>
   <si>
@@ -89,6 +74,21 @@
   </si>
   <si>
     <t>Mankind</t>
+  </si>
+  <si>
+    <t>Control ID</t>
+  </si>
+  <si>
+    <t>Control Description</t>
+  </si>
+  <si>
+    <t>Control Frequency</t>
+  </si>
+  <si>
+    <t>Control Type</t>
+  </si>
+  <si>
+    <t>Audit Leader From AE</t>
   </si>
 </sst>
 </file>
@@ -167,6 +167,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,162 +463,165 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>12651</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>11102</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>6463</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>7140</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>10575</v>
       </c>
       <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>4645</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>4310</v>
       </c>
       <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>3867</v>
       </c>
       <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>